<commit_message>
Fixed Phase 1 Instructions :)
</commit_message>
<xml_diff>
--- a/Phase2/Documentations/Phase 1 instructions.xlsx
+++ b/Phase2/Documentations/Phase 1 instructions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Pipeline-Processor\Phase2\Documentations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0733DA57-DD25-4892-8E02-F1048A4A9C86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EB496F4-5B77-4EF4-9A1E-9CC9BB249922}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -842,6 +842,27 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -857,12 +878,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -878,20 +893,83 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -899,89 +977,44 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -994,39 +1027,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1327,32 +1327,32 @@
       <c r="X1" s="1"/>
     </row>
     <row r="2" spans="3:24" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="C2" s="26"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="28" t="s">
-        <v>1</v>
-      </c>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28" t="s">
+      <c r="C2" s="14"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="28"/>
-      <c r="J2" s="28"/>
-      <c r="K2" s="29" t="s">
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="L2" s="28"/>
-      <c r="M2" s="28"/>
+      <c r="L2" s="16"/>
+      <c r="M2" s="16"/>
       <c r="N2" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="O2" s="28" t="s">
+      <c r="O2" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="P2" s="28"/>
-      <c r="Q2" s="28"/>
-      <c r="R2" s="30"/>
+      <c r="P2" s="16"/>
+      <c r="Q2" s="16"/>
+      <c r="R2" s="18"/>
     </row>
     <row r="3" spans="3:24" x14ac:dyDescent="0.35">
       <c r="C3" s="19" t="s">
@@ -1593,24 +1593,24 @@
       </c>
     </row>
     <row r="8" spans="3:24" x14ac:dyDescent="0.35">
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="D8" s="15"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="17"/>
-      <c r="I8" s="17"/>
-      <c r="J8" s="17"/>
-      <c r="K8" s="17"/>
-      <c r="L8" s="17"/>
-      <c r="M8" s="17"/>
-      <c r="N8" s="17"/>
-      <c r="O8" s="17"/>
-      <c r="P8" s="17"/>
-      <c r="Q8" s="17"/>
-      <c r="R8" s="18"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="24"/>
+      <c r="J8" s="24"/>
+      <c r="K8" s="24"/>
+      <c r="L8" s="24"/>
+      <c r="M8" s="24"/>
+      <c r="N8" s="24"/>
+      <c r="O8" s="24"/>
+      <c r="P8" s="24"/>
+      <c r="Q8" s="24"/>
+      <c r="R8" s="25"/>
     </row>
     <row r="9" spans="3:24" x14ac:dyDescent="0.35">
       <c r="C9" s="19" t="s">
@@ -1661,26 +1661,26 @@
       </c>
     </row>
     <row r="10" spans="3:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C10" s="21"/>
-      <c r="D10" s="22"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="24"/>
-      <c r="G10" s="22"/>
-      <c r="H10" s="23" t="s">
+      <c r="C10" s="26"/>
+      <c r="D10" s="27"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="29"/>
+      <c r="G10" s="27"/>
+      <c r="H10" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="I10" s="24"/>
-      <c r="J10" s="22"/>
-      <c r="K10" s="23" t="s">
+      <c r="I10" s="29"/>
+      <c r="J10" s="27"/>
+      <c r="K10" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="L10" s="24"/>
-      <c r="M10" s="22"/>
+      <c r="L10" s="29"/>
+      <c r="M10" s="27"/>
       <c r="N10" s="7"/>
-      <c r="O10" s="23"/>
-      <c r="P10" s="24"/>
-      <c r="Q10" s="24"/>
-      <c r="R10" s="25"/>
+      <c r="O10" s="28"/>
+      <c r="P10" s="29"/>
+      <c r="Q10" s="29"/>
+      <c r="R10" s="30"/>
     </row>
     <row r="11" spans="3:24" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="C11" s="9"/>
@@ -1821,16 +1821,6 @@
     <row r="30" spans="2:2" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="K2:M2"/>
-    <mergeCell ref="O2:R2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C7:D7"/>
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="E8:R8"/>
     <mergeCell ref="C9:D9"/>
@@ -1839,6 +1829,16 @@
     <mergeCell ref="H10:J10"/>
     <mergeCell ref="K10:M10"/>
     <mergeCell ref="O10:R10"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="K2:M2"/>
+    <mergeCell ref="O2:R2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1849,8 +1849,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0B95308-05A8-49F5-B594-EE21210B858B}">
   <dimension ref="B1:X39"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="I37" sqref="I37"/>
+    <sheetView topLeftCell="A19" zoomScale="90" workbookViewId="0">
+      <selection activeCell="H41" sqref="H41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1862,77 +1862,77 @@
   <sheetData>
     <row r="1" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="2:24" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="55" t="s">
+      <c r="B2" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="56"/>
-      <c r="D2" s="56"/>
-      <c r="E2" s="57"/>
-      <c r="F2" s="58" t="s">
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="G2" s="59"/>
-      <c r="H2" s="60"/>
-      <c r="K2" s="47" t="s">
+      <c r="G2" s="42"/>
+      <c r="H2" s="43"/>
+      <c r="K2" s="44" t="s">
         <v>39</v>
       </c>
-      <c r="L2" s="28"/>
-      <c r="M2" s="28"/>
-      <c r="N2" s="30"/>
-      <c r="O2" s="48" t="s">
+      <c r="L2" s="16"/>
+      <c r="M2" s="16"/>
+      <c r="N2" s="18"/>
+      <c r="O2" s="45" t="s">
         <v>31</v>
       </c>
-      <c r="P2" s="49"/>
-      <c r="Q2" s="50"/>
+      <c r="P2" s="46"/>
+      <c r="Q2" s="47"/>
     </row>
     <row r="3" spans="2:24" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="D3" s="15"/>
-      <c r="E3" s="44"/>
-      <c r="F3" s="54"/>
-      <c r="G3" s="54"/>
-      <c r="H3" s="54"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="34"/>
       <c r="K3" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="L3" s="15" t="s">
+      <c r="L3" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="M3" s="15"/>
-      <c r="N3" s="44"/>
-      <c r="O3" s="51" t="s">
+      <c r="M3" s="22"/>
+      <c r="N3" s="35"/>
+      <c r="O3" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="P3" s="52"/>
-      <c r="Q3" s="53"/>
+      <c r="P3" s="32"/>
+      <c r="Q3" s="33"/>
     </row>
     <row r="4" spans="2:24" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B4" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="D4" s="15"/>
-      <c r="E4" s="44"/>
-      <c r="F4" s="51" t="s">
+      <c r="D4" s="22"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="G4" s="52"/>
-      <c r="H4" s="53"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="33"/>
       <c r="K4" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="L4" s="15" t="s">
+      <c r="L4" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="M4" s="15"/>
-      <c r="N4" s="44"/>
+      <c r="M4" s="22"/>
+      <c r="N4" s="35"/>
       <c r="O4" s="5"/>
       <c r="P4" s="5"/>
       <c r="Q4" s="5"/>
@@ -1941,24 +1941,24 @@
       <c r="B5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="D5" s="15"/>
-      <c r="E5" s="44"/>
-      <c r="F5" s="51" t="s">
+      <c r="D5" s="22"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="G5" s="52"/>
-      <c r="H5" s="53"/>
+      <c r="G5" s="32"/>
+      <c r="H5" s="33"/>
       <c r="K5" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="L5" s="15" t="s">
+      <c r="L5" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="M5" s="15"/>
-      <c r="N5" s="44"/>
+      <c r="M5" s="22"/>
+      <c r="N5" s="35"/>
       <c r="O5" s="5"/>
       <c r="P5" s="5"/>
       <c r="Q5" s="5"/>
@@ -1967,22 +1967,22 @@
       <c r="B6" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="D6" s="15"/>
-      <c r="E6" s="44"/>
-      <c r="F6" s="51" t="s">
+      <c r="D6" s="22"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="G6" s="52"/>
-      <c r="H6" s="53"/>
+      <c r="G6" s="32"/>
+      <c r="H6" s="33"/>
       <c r="K6" s="2"/>
-      <c r="L6" s="15" t="s">
+      <c r="L6" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="M6" s="15"/>
-      <c r="N6" s="44"/>
+      <c r="M6" s="22"/>
+      <c r="N6" s="35"/>
       <c r="O6" s="5"/>
       <c r="P6" s="5"/>
       <c r="Q6" s="5"/>
@@ -1991,20 +1991,20 @@
       <c r="B7" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="D7" s="15"/>
-      <c r="E7" s="44"/>
-      <c r="F7" s="54"/>
-      <c r="G7" s="54"/>
-      <c r="H7" s="54"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="35"/>
+      <c r="F7" s="34"/>
+      <c r="G7" s="34"/>
+      <c r="H7" s="34"/>
       <c r="K7" s="2"/>
-      <c r="L7" s="15" t="s">
+      <c r="L7" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="M7" s="15"/>
-      <c r="N7" s="44"/>
+      <c r="M7" s="22"/>
+      <c r="N7" s="35"/>
       <c r="O7" s="5"/>
       <c r="P7" s="5"/>
       <c r="Q7" s="5"/>
@@ -2013,22 +2013,22 @@
       <c r="B8" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="D8" s="15"/>
-      <c r="E8" s="44"/>
-      <c r="F8" s="51" t="s">
+      <c r="D8" s="22"/>
+      <c r="E8" s="35"/>
+      <c r="F8" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="G8" s="52"/>
-      <c r="H8" s="53"/>
+      <c r="G8" s="32"/>
+      <c r="H8" s="33"/>
       <c r="K8" s="2"/>
-      <c r="L8" s="15" t="s">
+      <c r="L8" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="M8" s="15"/>
-      <c r="N8" s="44"/>
+      <c r="M8" s="22"/>
+      <c r="N8" s="35"/>
       <c r="O8" s="5"/>
       <c r="P8" s="5"/>
       <c r="Q8" s="5"/>
@@ -2037,22 +2037,22 @@
       <c r="B9" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C9" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="D9" s="15"/>
-      <c r="E9" s="44"/>
-      <c r="F9" s="54"/>
-      <c r="G9" s="54"/>
-      <c r="H9" s="54"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="35"/>
+      <c r="F9" s="34"/>
+      <c r="G9" s="34"/>
+      <c r="H9" s="34"/>
       <c r="K9" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="L9" s="15" t="s">
+      <c r="L9" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="M9" s="15"/>
-      <c r="N9" s="44"/>
+      <c r="M9" s="22"/>
+      <c r="N9" s="35"/>
       <c r="O9" s="5"/>
       <c r="P9" s="5"/>
       <c r="Q9" s="5"/>
@@ -2061,20 +2061,20 @@
       <c r="B10" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="45" t="s">
+      <c r="C10" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="D10" s="45"/>
-      <c r="E10" s="46"/>
-      <c r="F10" s="54"/>
-      <c r="G10" s="54"/>
-      <c r="H10" s="54"/>
+      <c r="D10" s="36"/>
+      <c r="E10" s="37"/>
+      <c r="F10" s="34"/>
+      <c r="G10" s="34"/>
+      <c r="H10" s="34"/>
       <c r="K10" s="6"/>
-      <c r="L10" s="45" t="s">
+      <c r="L10" s="36" t="s">
         <v>42</v>
       </c>
-      <c r="M10" s="45"/>
-      <c r="N10" s="46"/>
+      <c r="M10" s="36"/>
+      <c r="N10" s="37"/>
       <c r="O10" s="5"/>
       <c r="P10" s="5"/>
       <c r="Q10" s="5"/>
@@ -2082,52 +2082,52 @@
     <row r="11" spans="2:24" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
     <row r="15" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="16" spans="2:24" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="43" t="s">
+      <c r="B16" s="48" t="s">
         <v>47</v>
       </c>
-      <c r="C16" s="35"/>
-      <c r="D16" s="35"/>
-      <c r="E16" s="35"/>
-      <c r="F16" s="35"/>
-      <c r="G16" s="36"/>
-      <c r="I16" s="26"/>
-      <c r="J16" s="27"/>
-      <c r="K16" s="28" t="s">
-        <v>1</v>
-      </c>
-      <c r="L16" s="28"/>
-      <c r="M16" s="28"/>
-      <c r="N16" s="28" t="s">
+      <c r="C16" s="49"/>
+      <c r="D16" s="49"/>
+      <c r="E16" s="49"/>
+      <c r="F16" s="49"/>
+      <c r="G16" s="60"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="15"/>
+      <c r="K16" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="L16" s="16"/>
+      <c r="M16" s="16"/>
+      <c r="N16" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="O16" s="28"/>
-      <c r="P16" s="28"/>
-      <c r="Q16" s="29" t="s">
+      <c r="O16" s="16"/>
+      <c r="P16" s="16"/>
+      <c r="Q16" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="R16" s="28"/>
-      <c r="S16" s="28"/>
+      <c r="R16" s="16"/>
+      <c r="S16" s="16"/>
       <c r="T16" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="U16" s="28" t="s">
+      <c r="U16" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="V16" s="28"/>
-      <c r="W16" s="28"/>
-      <c r="X16" s="30"/>
+      <c r="V16" s="16"/>
+      <c r="W16" s="16"/>
+      <c r="X16" s="18"/>
     </row>
     <row r="17" spans="2:24" x14ac:dyDescent="0.35">
-      <c r="B17" s="40" t="s">
+      <c r="B17" s="50" t="s">
         <v>48</v>
       </c>
-      <c r="C17" s="41"/>
-      <c r="D17" s="41"/>
-      <c r="E17" s="37" t="s">
+      <c r="C17" s="51"/>
+      <c r="D17" s="51"/>
+      <c r="E17" s="52" t="s">
         <v>55</v>
       </c>
-      <c r="F17" s="37"/>
-      <c r="G17" s="38"/>
+      <c r="F17" s="52"/>
+      <c r="G17" s="53"/>
       <c r="H17" t="s">
         <v>73</v>
       </c>
@@ -2179,16 +2179,16 @@
       </c>
     </row>
     <row r="18" spans="2:24" x14ac:dyDescent="0.35">
-      <c r="B18" s="39" t="s">
+      <c r="B18" s="54" t="s">
         <v>49</v>
       </c>
-      <c r="C18" s="33"/>
-      <c r="D18" s="33"/>
-      <c r="E18" s="37" t="s">
+      <c r="C18" s="55"/>
+      <c r="D18" s="55"/>
+      <c r="E18" s="52" t="s">
         <v>56</v>
       </c>
-      <c r="F18" s="37"/>
-      <c r="G18" s="38"/>
+      <c r="F18" s="52"/>
+      <c r="G18" s="53"/>
       <c r="I18" s="19" t="s">
         <v>16</v>
       </c>
@@ -2237,16 +2237,16 @@
       </c>
     </row>
     <row r="19" spans="2:24" x14ac:dyDescent="0.35">
-      <c r="B19" s="39" t="s">
+      <c r="B19" s="54" t="s">
         <v>49</v>
       </c>
-      <c r="C19" s="33"/>
-      <c r="D19" s="33"/>
-      <c r="E19" s="37" t="s">
+      <c r="C19" s="55"/>
+      <c r="D19" s="55"/>
+      <c r="E19" s="52" t="s">
         <v>56</v>
       </c>
-      <c r="F19" s="37"/>
-      <c r="G19" s="38"/>
+      <c r="F19" s="52"/>
+      <c r="G19" s="53"/>
       <c r="I19" s="19" t="s">
         <v>19</v>
       </c>
@@ -2293,16 +2293,16 @@
       <c r="X19" s="4"/>
     </row>
     <row r="20" spans="2:24" x14ac:dyDescent="0.35">
-      <c r="B20" s="39" t="s">
+      <c r="B20" s="54" t="s">
         <v>49</v>
       </c>
-      <c r="C20" s="33"/>
-      <c r="D20" s="33"/>
-      <c r="E20" s="37" t="s">
+      <c r="C20" s="55"/>
+      <c r="D20" s="55"/>
+      <c r="E20" s="52" t="s">
         <v>56</v>
       </c>
-      <c r="F20" s="37"/>
-      <c r="G20" s="38"/>
+      <c r="F20" s="52"/>
+      <c r="G20" s="53"/>
       <c r="I20" s="19" t="s">
         <v>20</v>
       </c>
@@ -2351,16 +2351,16 @@
       </c>
     </row>
     <row r="21" spans="2:24" x14ac:dyDescent="0.35">
-      <c r="B21" s="39" t="s">
+      <c r="B21" s="54" t="s">
         <v>49</v>
       </c>
-      <c r="C21" s="33"/>
-      <c r="D21" s="33"/>
-      <c r="E21" s="37" t="s">
+      <c r="C21" s="55"/>
+      <c r="D21" s="55"/>
+      <c r="E21" s="52" t="s">
         <v>56</v>
       </c>
-      <c r="F21" s="37"/>
-      <c r="G21" s="38"/>
+      <c r="F21" s="52"/>
+      <c r="G21" s="53"/>
       <c r="I21" s="19" t="s">
         <v>66</v>
       </c>
@@ -2409,49 +2409,49 @@
       </c>
     </row>
     <row r="22" spans="2:24" x14ac:dyDescent="0.35">
-      <c r="B22" s="40" t="s">
+      <c r="B22" s="50" t="s">
         <v>50</v>
       </c>
-      <c r="C22" s="41"/>
-      <c r="D22" s="41"/>
-      <c r="E22" s="33" t="s">
+      <c r="C22" s="51"/>
+      <c r="D22" s="51"/>
+      <c r="E22" s="55" t="s">
         <v>57</v>
       </c>
-      <c r="F22" s="33"/>
-      <c r="G22" s="34"/>
+      <c r="F22" s="55"/>
+      <c r="G22" s="59"/>
       <c r="H22" t="s">
         <v>74</v>
       </c>
-      <c r="I22" s="14" t="s">
+      <c r="I22" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="J22" s="15"/>
-      <c r="K22" s="16"/>
-      <c r="L22" s="17"/>
-      <c r="M22" s="17"/>
-      <c r="N22" s="17"/>
-      <c r="O22" s="17"/>
-      <c r="P22" s="17"/>
-      <c r="Q22" s="17"/>
-      <c r="R22" s="17"/>
-      <c r="S22" s="17"/>
-      <c r="T22" s="17"/>
-      <c r="U22" s="17"/>
-      <c r="V22" s="17"/>
-      <c r="W22" s="17"/>
-      <c r="X22" s="18"/>
+      <c r="J22" s="22"/>
+      <c r="K22" s="23"/>
+      <c r="L22" s="24"/>
+      <c r="M22" s="24"/>
+      <c r="N22" s="24"/>
+      <c r="O22" s="24"/>
+      <c r="P22" s="24"/>
+      <c r="Q22" s="24"/>
+      <c r="R22" s="24"/>
+      <c r="S22" s="24"/>
+      <c r="T22" s="24"/>
+      <c r="U22" s="24"/>
+      <c r="V22" s="24"/>
+      <c r="W22" s="24"/>
+      <c r="X22" s="25"/>
     </row>
     <row r="23" spans="2:24" x14ac:dyDescent="0.35">
-      <c r="B23" s="39" t="s">
+      <c r="B23" s="54" t="s">
         <v>49</v>
       </c>
-      <c r="C23" s="33"/>
-      <c r="D23" s="33"/>
-      <c r="E23" s="37" t="s">
+      <c r="C23" s="55"/>
+      <c r="D23" s="55"/>
+      <c r="E23" s="52" t="s">
         <v>56</v>
       </c>
-      <c r="F23" s="37"/>
-      <c r="G23" s="38"/>
+      <c r="F23" s="52"/>
+      <c r="G23" s="53"/>
       <c r="I23" s="19" t="s">
         <v>21</v>
       </c>
@@ -2500,266 +2500,245 @@
       </c>
     </row>
     <row r="24" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B24" s="39" t="s">
+      <c r="B24" s="54" t="s">
         <v>49</v>
       </c>
-      <c r="C24" s="33"/>
-      <c r="D24" s="33"/>
-      <c r="E24" s="37" t="s">
+      <c r="C24" s="55"/>
+      <c r="D24" s="55"/>
+      <c r="E24" s="52" t="s">
         <v>56</v>
       </c>
-      <c r="F24" s="37"/>
-      <c r="G24" s="38"/>
-      <c r="I24" s="21"/>
-      <c r="J24" s="22"/>
-      <c r="K24" s="23"/>
-      <c r="L24" s="24"/>
-      <c r="M24" s="22"/>
-      <c r="N24" s="23" t="s">
+      <c r="F24" s="52"/>
+      <c r="G24" s="53"/>
+      <c r="I24" s="26"/>
+      <c r="J24" s="27"/>
+      <c r="K24" s="28"/>
+      <c r="L24" s="29"/>
+      <c r="M24" s="27"/>
+      <c r="N24" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="O24" s="24"/>
-      <c r="P24" s="22"/>
-      <c r="Q24" s="23" t="s">
+      <c r="O24" s="29"/>
+      <c r="P24" s="27"/>
+      <c r="Q24" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="R24" s="24"/>
-      <c r="S24" s="22"/>
+      <c r="R24" s="29"/>
+      <c r="S24" s="27"/>
       <c r="T24" s="7"/>
-      <c r="U24" s="23"/>
-      <c r="V24" s="24"/>
-      <c r="W24" s="24"/>
-      <c r="X24" s="25"/>
+      <c r="U24" s="28"/>
+      <c r="V24" s="29"/>
+      <c r="W24" s="29"/>
+      <c r="X24" s="30"/>
     </row>
     <row r="25" spans="2:24" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B25" s="39" t="s">
+      <c r="B25" s="54" t="s">
         <v>49</v>
       </c>
-      <c r="C25" s="33"/>
-      <c r="D25" s="33"/>
-      <c r="E25" s="37" t="s">
+      <c r="C25" s="55"/>
+      <c r="D25" s="55"/>
+      <c r="E25" s="52" t="s">
         <v>56</v>
       </c>
-      <c r="F25" s="37"/>
-      <c r="G25" s="38"/>
+      <c r="F25" s="52"/>
+      <c r="G25" s="53"/>
     </row>
     <row r="26" spans="2:24" x14ac:dyDescent="0.35">
-      <c r="B26" s="39" t="s">
+      <c r="B26" s="54" t="s">
         <v>49</v>
       </c>
-      <c r="C26" s="33"/>
-      <c r="D26" s="33"/>
-      <c r="E26" s="37" t="s">
+      <c r="C26" s="55"/>
+      <c r="D26" s="55"/>
+      <c r="E26" s="52" t="s">
         <v>56</v>
       </c>
-      <c r="F26" s="37"/>
-      <c r="G26" s="38"/>
+      <c r="F26" s="52"/>
+      <c r="G26" s="53"/>
     </row>
     <row r="27" spans="2:24" x14ac:dyDescent="0.35">
-      <c r="B27" s="40" t="s">
+      <c r="B27" s="50" t="s">
         <v>51</v>
       </c>
-      <c r="C27" s="41"/>
-      <c r="D27" s="41"/>
-      <c r="E27" s="33" t="s">
+      <c r="C27" s="51"/>
+      <c r="D27" s="51"/>
+      <c r="E27" s="55" t="s">
         <v>58</v>
       </c>
-      <c r="F27" s="33"/>
-      <c r="G27" s="34"/>
+      <c r="F27" s="55"/>
+      <c r="G27" s="59"/>
       <c r="H27" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="28" spans="2:24" x14ac:dyDescent="0.35">
-      <c r="B28" s="39" t="s">
+      <c r="B28" s="54" t="s">
         <v>49</v>
       </c>
-      <c r="C28" s="33"/>
-      <c r="D28" s="33"/>
-      <c r="E28" s="37" t="s">
+      <c r="C28" s="55"/>
+      <c r="D28" s="55"/>
+      <c r="E28" s="52" t="s">
         <v>56</v>
       </c>
-      <c r="F28" s="37"/>
-      <c r="G28" s="38"/>
+      <c r="F28" s="52"/>
+      <c r="G28" s="53"/>
     </row>
     <row r="29" spans="2:24" x14ac:dyDescent="0.35">
-      <c r="B29" s="39" t="s">
+      <c r="B29" s="54" t="s">
         <v>49</v>
       </c>
-      <c r="C29" s="33"/>
-      <c r="D29" s="33"/>
-      <c r="E29" s="37" t="s">
+      <c r="C29" s="55"/>
+      <c r="D29" s="55"/>
+      <c r="E29" s="52" t="s">
         <v>56</v>
       </c>
-      <c r="F29" s="37"/>
-      <c r="G29" s="38"/>
+      <c r="F29" s="52"/>
+      <c r="G29" s="53"/>
     </row>
     <row r="30" spans="2:24" x14ac:dyDescent="0.35">
-      <c r="B30" s="39" t="s">
+      <c r="B30" s="54" t="s">
         <v>49</v>
       </c>
-      <c r="C30" s="33"/>
-      <c r="D30" s="33"/>
-      <c r="E30" s="37" t="s">
+      <c r="C30" s="55"/>
+      <c r="D30" s="55"/>
+      <c r="E30" s="52" t="s">
         <v>56</v>
       </c>
-      <c r="F30" s="37"/>
-      <c r="G30" s="38"/>
+      <c r="F30" s="52"/>
+      <c r="G30" s="53"/>
     </row>
     <row r="31" spans="2:24" x14ac:dyDescent="0.35">
-      <c r="B31" s="39" t="s">
+      <c r="B31" s="54" t="s">
         <v>49</v>
       </c>
-      <c r="C31" s="33"/>
-      <c r="D31" s="33"/>
-      <c r="E31" s="37" t="s">
+      <c r="C31" s="55"/>
+      <c r="D31" s="55"/>
+      <c r="E31" s="52" t="s">
         <v>56</v>
       </c>
-      <c r="F31" s="37"/>
-      <c r="G31" s="38"/>
+      <c r="F31" s="52"/>
+      <c r="G31" s="53"/>
     </row>
     <row r="32" spans="2:24" x14ac:dyDescent="0.35">
-      <c r="B32" s="40" t="s">
+      <c r="B32" s="50" t="s">
         <v>52</v>
       </c>
-      <c r="C32" s="41"/>
-      <c r="D32" s="41"/>
-      <c r="E32" s="33" t="s">
+      <c r="C32" s="51"/>
+      <c r="D32" s="51"/>
+      <c r="E32" s="55" t="s">
         <v>59</v>
       </c>
-      <c r="F32" s="33"/>
-      <c r="G32" s="34"/>
+      <c r="F32" s="55"/>
+      <c r="G32" s="59"/>
       <c r="H32" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B33" s="39" t="s">
+      <c r="B33" s="54" t="s">
         <v>49</v>
       </c>
-      <c r="C33" s="33"/>
-      <c r="D33" s="33"/>
-      <c r="E33" s="37" t="s">
+      <c r="C33" s="55"/>
+      <c r="D33" s="55"/>
+      <c r="E33" s="52" t="s">
         <v>56</v>
       </c>
-      <c r="F33" s="37"/>
-      <c r="G33" s="38"/>
+      <c r="F33" s="52"/>
+      <c r="G33" s="53"/>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B34" s="39" t="s">
+      <c r="B34" s="54" t="s">
         <v>49</v>
       </c>
-      <c r="C34" s="33"/>
-      <c r="D34" s="33"/>
-      <c r="E34" s="37" t="s">
+      <c r="C34" s="55"/>
+      <c r="D34" s="55"/>
+      <c r="E34" s="52" t="s">
         <v>56</v>
       </c>
-      <c r="F34" s="37"/>
-      <c r="G34" s="38"/>
+      <c r="F34" s="52"/>
+      <c r="G34" s="53"/>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B35" s="39" t="s">
+      <c r="B35" s="54" t="s">
         <v>49</v>
       </c>
-      <c r="C35" s="33"/>
-      <c r="D35" s="33"/>
-      <c r="E35" s="37" t="s">
+      <c r="C35" s="55"/>
+      <c r="D35" s="55"/>
+      <c r="E35" s="52" t="s">
         <v>56</v>
       </c>
-      <c r="F35" s="37"/>
-      <c r="G35" s="38"/>
+      <c r="F35" s="52"/>
+      <c r="G35" s="53"/>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B36" s="39" t="s">
+      <c r="B36" s="54" t="s">
         <v>49</v>
       </c>
-      <c r="C36" s="33"/>
-      <c r="D36" s="33"/>
-      <c r="E36" s="37" t="s">
+      <c r="C36" s="55"/>
+      <c r="D36" s="55"/>
+      <c r="E36" s="52" t="s">
         <v>56</v>
       </c>
-      <c r="F36" s="37"/>
-      <c r="G36" s="38"/>
+      <c r="F36" s="52"/>
+      <c r="G36" s="53"/>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B37" s="40" t="s">
+      <c r="B37" s="50" t="s">
         <v>53</v>
       </c>
-      <c r="C37" s="41"/>
-      <c r="D37" s="41"/>
-      <c r="E37" s="33" t="s">
+      <c r="C37" s="51"/>
+      <c r="D37" s="51"/>
+      <c r="E37" s="55" t="s">
         <v>60</v>
       </c>
-      <c r="F37" s="33"/>
-      <c r="G37" s="34"/>
+      <c r="F37" s="55"/>
+      <c r="G37" s="59"/>
       <c r="H37" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="38" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B38" s="42" t="s">
+      <c r="B38" s="56" t="s">
         <v>54</v>
       </c>
-      <c r="C38" s="31"/>
-      <c r="D38" s="31"/>
-      <c r="E38" s="31" t="s">
+      <c r="C38" s="57"/>
+      <c r="D38" s="57"/>
+      <c r="E38" s="57" t="s">
         <v>54</v>
       </c>
-      <c r="F38" s="31"/>
-      <c r="G38" s="32"/>
+      <c r="F38" s="57"/>
+      <c r="G38" s="58"/>
     </row>
     <row r="39" spans="2:8" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="93">
-    <mergeCell ref="F8:H8"/>
-    <mergeCell ref="F9:H9"/>
-    <mergeCell ref="F10:H10"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="F3:H3"/>
-    <mergeCell ref="F4:H4"/>
-    <mergeCell ref="F5:H5"/>
-    <mergeCell ref="F6:H6"/>
-    <mergeCell ref="F7:H7"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="L3:N3"/>
-    <mergeCell ref="L5:N5"/>
-    <mergeCell ref="L4:N4"/>
-    <mergeCell ref="K2:N2"/>
-    <mergeCell ref="O2:Q2"/>
-    <mergeCell ref="O3:Q3"/>
-    <mergeCell ref="L6:N6"/>
-    <mergeCell ref="L7:N7"/>
-    <mergeCell ref="L8:N8"/>
-    <mergeCell ref="L9:N9"/>
-    <mergeCell ref="L10:N10"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="E17:G17"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="K24:M24"/>
+    <mergeCell ref="I24:J24"/>
+    <mergeCell ref="K22:X22"/>
+    <mergeCell ref="U24:X24"/>
+    <mergeCell ref="Q24:S24"/>
+    <mergeCell ref="N24:P24"/>
+    <mergeCell ref="Q16:S16"/>
+    <mergeCell ref="U16:X16"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="E38:G38"/>
+    <mergeCell ref="E37:G37"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="K16:M16"/>
+    <mergeCell ref="N16:P16"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="E33:G33"/>
+    <mergeCell ref="E34:G34"/>
+    <mergeCell ref="E35:G35"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="E22:G22"/>
+    <mergeCell ref="E27:G27"/>
+    <mergeCell ref="E32:G32"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="I22:J22"/>
     <mergeCell ref="B35:D35"/>
     <mergeCell ref="B36:D36"/>
     <mergeCell ref="B37:D37"/>
@@ -2776,34 +2755,55 @@
     <mergeCell ref="E29:G29"/>
     <mergeCell ref="E30:G30"/>
     <mergeCell ref="E31:G31"/>
-    <mergeCell ref="E38:G38"/>
-    <mergeCell ref="E37:G37"/>
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="K16:M16"/>
-    <mergeCell ref="N16:P16"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="E33:G33"/>
-    <mergeCell ref="E34:G34"/>
-    <mergeCell ref="E35:G35"/>
-    <mergeCell ref="E36:G36"/>
-    <mergeCell ref="E22:G22"/>
-    <mergeCell ref="E27:G27"/>
-    <mergeCell ref="E32:G32"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="K24:M24"/>
-    <mergeCell ref="I24:J24"/>
-    <mergeCell ref="K22:X22"/>
-    <mergeCell ref="U24:X24"/>
-    <mergeCell ref="Q24:S24"/>
-    <mergeCell ref="N24:P24"/>
-    <mergeCell ref="Q16:S16"/>
-    <mergeCell ref="U16:X16"/>
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="E17:G17"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="L6:N6"/>
+    <mergeCell ref="L7:N7"/>
+    <mergeCell ref="L8:N8"/>
+    <mergeCell ref="L9:N9"/>
+    <mergeCell ref="L10:N10"/>
+    <mergeCell ref="L3:N3"/>
+    <mergeCell ref="L5:N5"/>
+    <mergeCell ref="L4:N4"/>
+    <mergeCell ref="K2:N2"/>
+    <mergeCell ref="O2:Q2"/>
+    <mergeCell ref="O3:Q3"/>
+    <mergeCell ref="F6:H6"/>
+    <mergeCell ref="F7:H7"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="F8:H8"/>
+    <mergeCell ref="F9:H9"/>
+    <mergeCell ref="F10:H10"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="C10:E10"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2815,8 +2815,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F814EA7-F7BF-4632-9048-BF344D7277A4}">
   <dimension ref="B1:AD44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N4" workbookViewId="0">
-      <selection activeCell="O20" sqref="O20:P20"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="54" workbookViewId="0">
+      <selection activeCell="T36" sqref="T36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2827,153 +2827,153 @@
   <sheetData>
     <row r="1" spans="2:30" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="2:30" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="55" t="s">
+      <c r="B2" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="56"/>
-      <c r="D2" s="56"/>
-      <c r="E2" s="72"/>
-      <c r="F2" s="58" t="s">
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="67"/>
+      <c r="F2" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="G2" s="59"/>
-      <c r="H2" s="59"/>
-      <c r="I2" s="59"/>
-      <c r="J2" s="59"/>
-      <c r="K2" s="59"/>
-      <c r="L2" s="59"/>
-      <c r="M2" s="59"/>
-      <c r="N2" s="60"/>
-      <c r="Q2" s="47" t="s">
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="42"/>
+      <c r="K2" s="42"/>
+      <c r="L2" s="42"/>
+      <c r="M2" s="42"/>
+      <c r="N2" s="43"/>
+      <c r="Q2" s="44" t="s">
         <v>39</v>
       </c>
-      <c r="R2" s="28"/>
-      <c r="S2" s="28"/>
-      <c r="T2" s="30"/>
-      <c r="U2" s="73" t="s">
+      <c r="R2" s="16"/>
+      <c r="S2" s="16"/>
+      <c r="T2" s="18"/>
+      <c r="U2" s="68" t="s">
         <v>31</v>
       </c>
-      <c r="V2" s="74"/>
-      <c r="W2" s="75"/>
+      <c r="V2" s="69"/>
+      <c r="W2" s="70"/>
     </row>
     <row r="3" spans="2:30" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="D3" s="15"/>
-      <c r="E3" s="44"/>
-      <c r="F3" s="65"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="65"/>
-      <c r="I3" s="65"/>
-      <c r="J3" s="65"/>
-      <c r="K3" s="65"/>
-      <c r="L3" s="65"/>
-      <c r="M3" s="65"/>
-      <c r="N3" s="65"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="71"/>
+      <c r="G3" s="71"/>
+      <c r="H3" s="71"/>
+      <c r="I3" s="71"/>
+      <c r="J3" s="71"/>
+      <c r="K3" s="71"/>
+      <c r="L3" s="71"/>
+      <c r="M3" s="71"/>
+      <c r="N3" s="71"/>
       <c r="Q3" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="R3" s="15" t="s">
+      <c r="R3" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="S3" s="15"/>
-      <c r="T3" s="44"/>
+      <c r="S3" s="22"/>
+      <c r="T3" s="35"/>
     </row>
     <row r="4" spans="2:30" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B4" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="D4" s="15"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="66" t="s">
+      <c r="D4" s="22"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="61" t="s">
         <v>32</v>
       </c>
-      <c r="G4" s="67"/>
-      <c r="H4" s="68"/>
-      <c r="I4" s="66" t="s">
+      <c r="G4" s="62"/>
+      <c r="H4" s="63"/>
+      <c r="I4" s="61" t="s">
         <v>34</v>
       </c>
-      <c r="J4" s="67"/>
-      <c r="K4" s="68"/>
-      <c r="L4" s="69" t="s">
+      <c r="J4" s="62"/>
+      <c r="K4" s="63"/>
+      <c r="L4" s="64" t="s">
         <v>72</v>
       </c>
-      <c r="M4" s="70"/>
-      <c r="N4" s="71"/>
+      <c r="M4" s="65"/>
+      <c r="N4" s="66"/>
       <c r="Q4" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="R4" s="15" t="s">
+      <c r="R4" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="S4" s="15"/>
-      <c r="T4" s="44"/>
+      <c r="S4" s="22"/>
+      <c r="T4" s="35"/>
     </row>
     <row r="5" spans="2:30" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="D5" s="15"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="69" t="s">
+      <c r="D5" s="22"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="64" t="s">
         <v>33</v>
       </c>
-      <c r="G5" s="70"/>
-      <c r="H5" s="71"/>
-      <c r="I5" s="65"/>
-      <c r="J5" s="65"/>
-      <c r="K5" s="65"/>
-      <c r="L5" s="65"/>
-      <c r="M5" s="65"/>
-      <c r="N5" s="65"/>
+      <c r="G5" s="65"/>
+      <c r="H5" s="66"/>
+      <c r="I5" s="71"/>
+      <c r="J5" s="71"/>
+      <c r="K5" s="71"/>
+      <c r="L5" s="71"/>
+      <c r="M5" s="71"/>
+      <c r="N5" s="71"/>
       <c r="Q5" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="R5" s="15" t="s">
+      <c r="R5" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="S5" s="15"/>
-      <c r="T5" s="44"/>
-      <c r="U5" s="51" t="s">
+      <c r="S5" s="22"/>
+      <c r="T5" s="35"/>
+      <c r="U5" s="31" t="s">
         <v>72</v>
       </c>
-      <c r="V5" s="52"/>
-      <c r="W5" s="53"/>
+      <c r="V5" s="32"/>
+      <c r="W5" s="33"/>
     </row>
     <row r="6" spans="2:30" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B6" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="D6" s="15"/>
-      <c r="E6" s="44"/>
-      <c r="F6" s="65"/>
-      <c r="G6" s="65"/>
-      <c r="H6" s="65"/>
-      <c r="I6" s="65"/>
-      <c r="J6" s="65"/>
-      <c r="K6" s="65"/>
-      <c r="L6" s="65"/>
-      <c r="M6" s="65"/>
-      <c r="N6" s="65"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="71"/>
+      <c r="G6" s="71"/>
+      <c r="H6" s="71"/>
+      <c r="I6" s="71"/>
+      <c r="J6" s="71"/>
+      <c r="K6" s="71"/>
+      <c r="L6" s="71"/>
+      <c r="M6" s="71"/>
+      <c r="N6" s="71"/>
       <c r="Q6" s="2"/>
-      <c r="R6" s="15" t="s">
+      <c r="R6" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="S6" s="15"/>
-      <c r="T6" s="44"/>
+      <c r="S6" s="22"/>
+      <c r="T6" s="35"/>
       <c r="U6" s="5"/>
       <c r="V6" s="5"/>
       <c r="W6" s="5"/>
@@ -2982,26 +2982,26 @@
       <c r="B7" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="D7" s="15"/>
-      <c r="E7" s="44"/>
-      <c r="F7" s="65"/>
-      <c r="G7" s="65"/>
-      <c r="H7" s="65"/>
-      <c r="I7" s="65"/>
-      <c r="J7" s="65"/>
-      <c r="K7" s="65"/>
-      <c r="L7" s="65"/>
-      <c r="M7" s="65"/>
-      <c r="N7" s="65"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="35"/>
+      <c r="F7" s="71"/>
+      <c r="G7" s="71"/>
+      <c r="H7" s="71"/>
+      <c r="I7" s="71"/>
+      <c r="J7" s="71"/>
+      <c r="K7" s="71"/>
+      <c r="L7" s="71"/>
+      <c r="M7" s="71"/>
+      <c r="N7" s="71"/>
       <c r="Q7" s="2"/>
-      <c r="R7" s="15" t="s">
+      <c r="R7" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="S7" s="15"/>
-      <c r="T7" s="44"/>
+      <c r="S7" s="22"/>
+      <c r="T7" s="35"/>
       <c r="U7" s="5"/>
       <c r="V7" s="5"/>
       <c r="W7" s="5"/>
@@ -3010,26 +3010,26 @@
       <c r="B8" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="D8" s="15"/>
-      <c r="E8" s="44"/>
-      <c r="F8" s="65"/>
-      <c r="G8" s="65"/>
-      <c r="H8" s="65"/>
-      <c r="I8" s="65"/>
-      <c r="J8" s="65"/>
-      <c r="K8" s="65"/>
-      <c r="L8" s="65"/>
-      <c r="M8" s="65"/>
-      <c r="N8" s="65"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="35"/>
+      <c r="F8" s="71"/>
+      <c r="G8" s="71"/>
+      <c r="H8" s="71"/>
+      <c r="I8" s="71"/>
+      <c r="J8" s="71"/>
+      <c r="K8" s="71"/>
+      <c r="L8" s="71"/>
+      <c r="M8" s="71"/>
+      <c r="N8" s="71"/>
       <c r="Q8" s="2"/>
-      <c r="R8" s="15" t="s">
+      <c r="R8" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="S8" s="15"/>
-      <c r="T8" s="44"/>
+      <c r="S8" s="22"/>
+      <c r="T8" s="35"/>
       <c r="U8" s="5"/>
       <c r="V8" s="5"/>
       <c r="W8" s="5"/>
@@ -3038,28 +3038,28 @@
       <c r="B9" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C9" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="D9" s="15"/>
-      <c r="E9" s="44"/>
-      <c r="F9" s="65"/>
-      <c r="G9" s="65"/>
-      <c r="H9" s="65"/>
-      <c r="I9" s="65"/>
-      <c r="J9" s="65"/>
-      <c r="K9" s="65"/>
-      <c r="L9" s="65"/>
-      <c r="M9" s="65"/>
-      <c r="N9" s="65"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="35"/>
+      <c r="F9" s="71"/>
+      <c r="G9" s="71"/>
+      <c r="H9" s="71"/>
+      <c r="I9" s="71"/>
+      <c r="J9" s="71"/>
+      <c r="K9" s="71"/>
+      <c r="L9" s="71"/>
+      <c r="M9" s="71"/>
+      <c r="N9" s="71"/>
       <c r="Q9" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="R9" s="15" t="s">
+      <c r="R9" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="S9" s="15"/>
-      <c r="T9" s="44"/>
+      <c r="S9" s="22"/>
+      <c r="T9" s="35"/>
       <c r="U9" s="5"/>
       <c r="V9" s="5"/>
       <c r="W9" s="5"/>
@@ -3068,26 +3068,26 @@
       <c r="B10" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="45" t="s">
+      <c r="C10" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="D10" s="45"/>
-      <c r="E10" s="46"/>
-      <c r="F10" s="65"/>
-      <c r="G10" s="65"/>
-      <c r="H10" s="65"/>
-      <c r="I10" s="65"/>
-      <c r="J10" s="65"/>
-      <c r="K10" s="65"/>
-      <c r="L10" s="65"/>
-      <c r="M10" s="65"/>
-      <c r="N10" s="65"/>
+      <c r="D10" s="36"/>
+      <c r="E10" s="37"/>
+      <c r="F10" s="71"/>
+      <c r="G10" s="71"/>
+      <c r="H10" s="71"/>
+      <c r="I10" s="71"/>
+      <c r="J10" s="71"/>
+      <c r="K10" s="71"/>
+      <c r="L10" s="71"/>
+      <c r="M10" s="71"/>
+      <c r="N10" s="71"/>
       <c r="Q10" s="6"/>
-      <c r="R10" s="45" t="s">
+      <c r="R10" s="36" t="s">
         <v>42</v>
       </c>
-      <c r="S10" s="45"/>
-      <c r="T10" s="46"/>
+      <c r="S10" s="36"/>
+      <c r="T10" s="37"/>
       <c r="U10" s="5"/>
       <c r="V10" s="5"/>
       <c r="W10" s="5"/>
@@ -3095,52 +3095,52 @@
     <row r="11" spans="2:30" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
     <row r="15" spans="2:30" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="16" spans="2:30" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="43" t="s">
+      <c r="B16" s="48" t="s">
         <v>47</v>
       </c>
-      <c r="C16" s="35"/>
-      <c r="D16" s="35"/>
-      <c r="E16" s="35"/>
-      <c r="F16" s="35"/>
-      <c r="G16" s="36"/>
-      <c r="O16" s="26"/>
-      <c r="P16" s="27"/>
-      <c r="Q16" s="28" t="s">
-        <v>1</v>
-      </c>
-      <c r="R16" s="28"/>
-      <c r="S16" s="28"/>
-      <c r="T16" s="28" t="s">
+      <c r="C16" s="49"/>
+      <c r="D16" s="49"/>
+      <c r="E16" s="49"/>
+      <c r="F16" s="49"/>
+      <c r="G16" s="60"/>
+      <c r="O16" s="14"/>
+      <c r="P16" s="15"/>
+      <c r="Q16" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="R16" s="16"/>
+      <c r="S16" s="16"/>
+      <c r="T16" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="U16" s="28"/>
-      <c r="V16" s="28"/>
-      <c r="W16" s="29" t="s">
+      <c r="U16" s="16"/>
+      <c r="V16" s="16"/>
+      <c r="W16" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="X16" s="28"/>
-      <c r="Y16" s="28"/>
+      <c r="X16" s="16"/>
+      <c r="Y16" s="16"/>
       <c r="Z16" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="AA16" s="28" t="s">
+      <c r="AA16" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="AB16" s="28"/>
-      <c r="AC16" s="28"/>
-      <c r="AD16" s="30"/>
+      <c r="AB16" s="16"/>
+      <c r="AC16" s="16"/>
+      <c r="AD16" s="18"/>
     </row>
     <row r="17" spans="2:30" x14ac:dyDescent="0.35">
-      <c r="B17" s="40" t="s">
+      <c r="B17" s="50" t="s">
         <v>78</v>
       </c>
-      <c r="C17" s="41"/>
-      <c r="D17" s="41"/>
-      <c r="E17" s="37" t="s">
+      <c r="C17" s="51"/>
+      <c r="D17" s="51"/>
+      <c r="E17" s="52" t="s">
         <v>79</v>
       </c>
-      <c r="F17" s="37"/>
-      <c r="G17" s="38"/>
+      <c r="F17" s="52"/>
+      <c r="G17" s="53"/>
       <c r="O17" s="19" t="s">
         <v>0</v>
       </c>
@@ -3189,16 +3189,16 @@
       </c>
     </row>
     <row r="18" spans="2:30" x14ac:dyDescent="0.35">
-      <c r="B18" s="40" t="s">
+      <c r="B18" s="50" t="s">
         <v>32</v>
       </c>
-      <c r="C18" s="41"/>
-      <c r="D18" s="41"/>
-      <c r="E18" s="37" t="s">
+      <c r="C18" s="51"/>
+      <c r="D18" s="51"/>
+      <c r="E18" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="F18" s="37"/>
-      <c r="G18" s="38"/>
+      <c r="F18" s="52"/>
+      <c r="G18" s="53"/>
       <c r="O18" s="19" t="s">
         <v>16</v>
       </c>
@@ -3247,16 +3247,16 @@
       </c>
     </row>
     <row r="19" spans="2:30" x14ac:dyDescent="0.35">
-      <c r="B19" s="39" t="s">
+      <c r="B19" s="54" t="s">
         <v>49</v>
       </c>
-      <c r="C19" s="33"/>
-      <c r="D19" s="33"/>
-      <c r="E19" s="37" t="s">
+      <c r="C19" s="55"/>
+      <c r="D19" s="55"/>
+      <c r="E19" s="52" t="s">
         <v>56</v>
       </c>
-      <c r="F19" s="37"/>
-      <c r="G19" s="38"/>
+      <c r="F19" s="52"/>
+      <c r="G19" s="53"/>
       <c r="O19" s="19" t="s">
         <v>19</v>
       </c>
@@ -3303,16 +3303,16 @@
       <c r="AD19" s="4"/>
     </row>
     <row r="20" spans="2:30" x14ac:dyDescent="0.35">
-      <c r="B20" s="39" t="s">
+      <c r="B20" s="54" t="s">
         <v>49</v>
       </c>
-      <c r="C20" s="33"/>
-      <c r="D20" s="33"/>
-      <c r="E20" s="37" t="s">
+      <c r="C20" s="55"/>
+      <c r="D20" s="55"/>
+      <c r="E20" s="52" t="s">
         <v>56</v>
       </c>
-      <c r="F20" s="37"/>
-      <c r="G20" s="38"/>
+      <c r="F20" s="52"/>
+      <c r="G20" s="53"/>
       <c r="O20" s="19" t="s">
         <v>20</v>
       </c>
@@ -3361,16 +3361,16 @@
       </c>
     </row>
     <row r="21" spans="2:30" x14ac:dyDescent="0.35">
-      <c r="B21" s="39" t="s">
+      <c r="B21" s="54" t="s">
         <v>49</v>
       </c>
-      <c r="C21" s="33"/>
-      <c r="D21" s="33"/>
-      <c r="E21" s="37" t="s">
+      <c r="C21" s="55"/>
+      <c r="D21" s="55"/>
+      <c r="E21" s="52" t="s">
         <v>56</v>
       </c>
-      <c r="F21" s="37"/>
-      <c r="G21" s="38"/>
+      <c r="F21" s="52"/>
+      <c r="G21" s="53"/>
       <c r="O21" s="19" t="s">
         <v>66</v>
       </c>
@@ -3419,46 +3419,46 @@
       </c>
     </row>
     <row r="22" spans="2:30" x14ac:dyDescent="0.35">
-      <c r="B22" s="39" t="s">
+      <c r="B22" s="54" t="s">
         <v>49</v>
       </c>
-      <c r="C22" s="33"/>
-      <c r="D22" s="33"/>
-      <c r="E22" s="37" t="s">
+      <c r="C22" s="55"/>
+      <c r="D22" s="55"/>
+      <c r="E22" s="52" t="s">
         <v>56</v>
       </c>
-      <c r="F22" s="37"/>
-      <c r="G22" s="38"/>
-      <c r="O22" s="14" t="s">
+      <c r="F22" s="52"/>
+      <c r="G22" s="53"/>
+      <c r="O22" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="P22" s="15"/>
-      <c r="Q22" s="16"/>
-      <c r="R22" s="17"/>
-      <c r="S22" s="17"/>
-      <c r="T22" s="17"/>
-      <c r="U22" s="17"/>
-      <c r="V22" s="17"/>
-      <c r="W22" s="17"/>
-      <c r="X22" s="17"/>
-      <c r="Y22" s="17"/>
-      <c r="Z22" s="17"/>
-      <c r="AA22" s="17"/>
-      <c r="AB22" s="17"/>
-      <c r="AC22" s="17"/>
-      <c r="AD22" s="18"/>
+      <c r="P22" s="22"/>
+      <c r="Q22" s="23"/>
+      <c r="R22" s="24"/>
+      <c r="S22" s="24"/>
+      <c r="T22" s="24"/>
+      <c r="U22" s="24"/>
+      <c r="V22" s="24"/>
+      <c r="W22" s="24"/>
+      <c r="X22" s="24"/>
+      <c r="Y22" s="24"/>
+      <c r="Z22" s="24"/>
+      <c r="AA22" s="24"/>
+      <c r="AB22" s="24"/>
+      <c r="AC22" s="24"/>
+      <c r="AD22" s="25"/>
     </row>
     <row r="23" spans="2:30" x14ac:dyDescent="0.35">
-      <c r="B23" s="40" t="s">
+      <c r="B23" s="50" t="s">
         <v>80</v>
       </c>
-      <c r="C23" s="41"/>
-      <c r="D23" s="41"/>
-      <c r="E23" s="37" t="s">
+      <c r="C23" s="51"/>
+      <c r="D23" s="51"/>
+      <c r="E23" s="52" t="s">
         <v>81</v>
       </c>
-      <c r="F23" s="37"/>
-      <c r="G23" s="38"/>
+      <c r="F23" s="52"/>
+      <c r="G23" s="53"/>
       <c r="O23" s="19" t="s">
         <v>21</v>
       </c>
@@ -3507,378 +3507,279 @@
       </c>
     </row>
     <row r="24" spans="2:30" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B24" s="40" t="s">
+      <c r="B24" s="50" t="s">
         <v>33</v>
       </c>
-      <c r="C24" s="41"/>
-      <c r="D24" s="41"/>
-      <c r="E24" s="37" t="s">
+      <c r="C24" s="51"/>
+      <c r="D24" s="51"/>
+      <c r="E24" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="F24" s="37"/>
-      <c r="G24" s="38"/>
-      <c r="O24" s="21"/>
-      <c r="P24" s="22"/>
-      <c r="Q24" s="23"/>
-      <c r="R24" s="24"/>
-      <c r="S24" s="22"/>
-      <c r="T24" s="23" t="s">
+      <c r="F24" s="52"/>
+      <c r="G24" s="53"/>
+      <c r="O24" s="26"/>
+      <c r="P24" s="27"/>
+      <c r="Q24" s="28"/>
+      <c r="R24" s="29"/>
+      <c r="S24" s="27"/>
+      <c r="T24" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="U24" s="24"/>
-      <c r="V24" s="22"/>
-      <c r="W24" s="23" t="s">
+      <c r="U24" s="29"/>
+      <c r="V24" s="27"/>
+      <c r="W24" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="X24" s="24"/>
-      <c r="Y24" s="22"/>
+      <c r="X24" s="29"/>
+      <c r="Y24" s="27"/>
       <c r="Z24" s="7"/>
-      <c r="AA24" s="23"/>
-      <c r="AB24" s="24"/>
-      <c r="AC24" s="24"/>
-      <c r="AD24" s="25"/>
+      <c r="AA24" s="28"/>
+      <c r="AB24" s="29"/>
+      <c r="AC24" s="29"/>
+      <c r="AD24" s="30"/>
     </row>
     <row r="25" spans="2:30" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B25" s="39" t="s">
+      <c r="B25" s="54" t="s">
         <v>49</v>
       </c>
-      <c r="C25" s="33"/>
-      <c r="D25" s="33"/>
-      <c r="E25" s="37" t="s">
+      <c r="C25" s="55"/>
+      <c r="D25" s="55"/>
+      <c r="E25" s="52" t="s">
         <v>56</v>
       </c>
-      <c r="F25" s="37"/>
-      <c r="G25" s="38"/>
+      <c r="F25" s="52"/>
+      <c r="G25" s="53"/>
     </row>
     <row r="26" spans="2:30" x14ac:dyDescent="0.35">
-      <c r="B26" s="39" t="s">
+      <c r="B26" s="54" t="s">
         <v>49</v>
       </c>
-      <c r="C26" s="33"/>
-      <c r="D26" s="33"/>
-      <c r="E26" s="37" t="s">
+      <c r="C26" s="55"/>
+      <c r="D26" s="55"/>
+      <c r="E26" s="52" t="s">
         <v>56</v>
       </c>
-      <c r="F26" s="37"/>
-      <c r="G26" s="38"/>
+      <c r="F26" s="52"/>
+      <c r="G26" s="53"/>
     </row>
     <row r="27" spans="2:30" x14ac:dyDescent="0.35">
-      <c r="B27" s="39" t="s">
+      <c r="B27" s="54" t="s">
         <v>49</v>
       </c>
-      <c r="C27" s="33"/>
-      <c r="D27" s="33"/>
-      <c r="E27" s="37" t="s">
+      <c r="C27" s="55"/>
+      <c r="D27" s="55"/>
+      <c r="E27" s="52" t="s">
         <v>56</v>
       </c>
-      <c r="F27" s="37"/>
-      <c r="G27" s="38"/>
+      <c r="F27" s="52"/>
+      <c r="G27" s="53"/>
     </row>
     <row r="28" spans="2:30" x14ac:dyDescent="0.35">
-      <c r="B28" s="39" t="s">
+      <c r="B28" s="54" t="s">
         <v>49</v>
       </c>
-      <c r="C28" s="33"/>
-      <c r="D28" s="33"/>
-      <c r="E28" s="37" t="s">
+      <c r="C28" s="55"/>
+      <c r="D28" s="55"/>
+      <c r="E28" s="52" t="s">
         <v>56</v>
       </c>
-      <c r="F28" s="37"/>
-      <c r="G28" s="38"/>
+      <c r="F28" s="52"/>
+      <c r="G28" s="53"/>
     </row>
     <row r="29" spans="2:30" x14ac:dyDescent="0.35">
-      <c r="B29" s="40" t="s">
+      <c r="B29" s="50" t="s">
         <v>49</v>
       </c>
-      <c r="C29" s="41"/>
-      <c r="D29" s="41"/>
-      <c r="E29" s="37" t="s">
+      <c r="C29" s="51"/>
+      <c r="D29" s="51"/>
+      <c r="E29" s="52" t="s">
         <v>56</v>
       </c>
-      <c r="F29" s="37"/>
-      <c r="G29" s="38"/>
+      <c r="F29" s="52"/>
+      <c r="G29" s="53"/>
     </row>
     <row r="30" spans="2:30" x14ac:dyDescent="0.35">
-      <c r="B30" s="39" t="s">
+      <c r="B30" s="54" t="s">
         <v>49</v>
       </c>
-      <c r="C30" s="33"/>
-      <c r="D30" s="33"/>
-      <c r="E30" s="37" t="s">
+      <c r="C30" s="55"/>
+      <c r="D30" s="55"/>
+      <c r="E30" s="52" t="s">
         <v>56</v>
       </c>
-      <c r="F30" s="37"/>
-      <c r="G30" s="38"/>
+      <c r="F30" s="52"/>
+      <c r="G30" s="53"/>
     </row>
     <row r="31" spans="2:30" x14ac:dyDescent="0.35">
-      <c r="B31" s="39" t="s">
+      <c r="B31" s="54" t="s">
         <v>49</v>
       </c>
-      <c r="C31" s="33"/>
-      <c r="D31" s="33"/>
-      <c r="E31" s="37" t="s">
+      <c r="C31" s="55"/>
+      <c r="D31" s="55"/>
+      <c r="E31" s="52" t="s">
         <v>56</v>
       </c>
-      <c r="F31" s="37"/>
-      <c r="G31" s="38"/>
+      <c r="F31" s="52"/>
+      <c r="G31" s="53"/>
     </row>
     <row r="32" spans="2:30" x14ac:dyDescent="0.35">
-      <c r="B32" s="39" t="s">
+      <c r="B32" s="54" t="s">
         <v>49</v>
       </c>
-      <c r="C32" s="33"/>
-      <c r="D32" s="33"/>
-      <c r="E32" s="37" t="s">
+      <c r="C32" s="55"/>
+      <c r="D32" s="55"/>
+      <c r="E32" s="52" t="s">
         <v>56</v>
       </c>
-      <c r="F32" s="37"/>
-      <c r="G32" s="38"/>
+      <c r="F32" s="52"/>
+      <c r="G32" s="53"/>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B33" s="39" t="s">
+      <c r="B33" s="54" t="s">
         <v>49</v>
       </c>
-      <c r="C33" s="33"/>
-      <c r="D33" s="33"/>
-      <c r="E33" s="37" t="s">
+      <c r="C33" s="55"/>
+      <c r="D33" s="55"/>
+      <c r="E33" s="52" t="s">
         <v>56</v>
       </c>
-      <c r="F33" s="37"/>
-      <c r="G33" s="38"/>
+      <c r="F33" s="52"/>
+      <c r="G33" s="53"/>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B34" s="40" t="s">
+      <c r="B34" s="50" t="s">
         <v>82</v>
       </c>
-      <c r="C34" s="41"/>
-      <c r="D34" s="41"/>
-      <c r="E34" s="37" t="s">
+      <c r="C34" s="51"/>
+      <c r="D34" s="51"/>
+      <c r="E34" s="52" t="s">
         <v>83</v>
       </c>
-      <c r="F34" s="37"/>
-      <c r="G34" s="38"/>
+      <c r="F34" s="52"/>
+      <c r="G34" s="53"/>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B35" s="39" t="s">
+      <c r="B35" s="54" t="s">
         <v>49</v>
       </c>
-      <c r="C35" s="33"/>
-      <c r="D35" s="33"/>
-      <c r="E35" s="37" t="s">
+      <c r="C35" s="55"/>
+      <c r="D35" s="55"/>
+      <c r="E35" s="52" t="s">
         <v>56</v>
       </c>
-      <c r="F35" s="37"/>
-      <c r="G35" s="38"/>
+      <c r="F35" s="52"/>
+      <c r="G35" s="53"/>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B36" s="39" t="s">
+      <c r="B36" s="54" t="s">
         <v>49</v>
       </c>
-      <c r="C36" s="33"/>
-      <c r="D36" s="33"/>
-      <c r="E36" s="37" t="s">
+      <c r="C36" s="55"/>
+      <c r="D36" s="55"/>
+      <c r="E36" s="52" t="s">
         <v>56</v>
       </c>
-      <c r="F36" s="37"/>
-      <c r="G36" s="38"/>
+      <c r="F36" s="52"/>
+      <c r="G36" s="53"/>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B37" s="39" t="s">
+      <c r="B37" s="54" t="s">
         <v>49</v>
       </c>
-      <c r="C37" s="33"/>
-      <c r="D37" s="33"/>
-      <c r="E37" s="37" t="s">
+      <c r="C37" s="55"/>
+      <c r="D37" s="55"/>
+      <c r="E37" s="52" t="s">
         <v>56</v>
       </c>
-      <c r="F37" s="37"/>
-      <c r="G37" s="38"/>
+      <c r="F37" s="52"/>
+      <c r="G37" s="53"/>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B38" s="39" t="s">
+      <c r="B38" s="54" t="s">
         <v>49</v>
       </c>
-      <c r="C38" s="33"/>
-      <c r="D38" s="33"/>
-      <c r="E38" s="37" t="s">
+      <c r="C38" s="55"/>
+      <c r="D38" s="55"/>
+      <c r="E38" s="52" t="s">
         <v>56</v>
       </c>
-      <c r="F38" s="37"/>
-      <c r="G38" s="38"/>
+      <c r="F38" s="52"/>
+      <c r="G38" s="53"/>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B39" s="40" t="s">
+      <c r="B39" s="50" t="s">
         <v>84</v>
       </c>
-      <c r="C39" s="41"/>
-      <c r="D39" s="41"/>
-      <c r="E39" s="37" t="s">
+      <c r="C39" s="51"/>
+      <c r="D39" s="51"/>
+      <c r="E39" s="52" t="s">
         <v>85</v>
       </c>
-      <c r="F39" s="37"/>
-      <c r="G39" s="38"/>
+      <c r="F39" s="52"/>
+      <c r="G39" s="53"/>
     </row>
     <row r="40" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B40" s="39" t="s">
+      <c r="B40" s="54" t="s">
         <v>49</v>
       </c>
-      <c r="C40" s="33"/>
-      <c r="D40" s="33"/>
-      <c r="E40" s="37" t="s">
+      <c r="C40" s="55"/>
+      <c r="D40" s="55"/>
+      <c r="E40" s="52" t="s">
         <v>56</v>
       </c>
-      <c r="F40" s="37"/>
-      <c r="G40" s="38"/>
+      <c r="F40" s="52"/>
+      <c r="G40" s="53"/>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B41" s="39" t="s">
+      <c r="B41" s="54" t="s">
         <v>49</v>
       </c>
-      <c r="C41" s="33"/>
-      <c r="D41" s="33"/>
-      <c r="E41" s="37" t="s">
+      <c r="C41" s="55"/>
+      <c r="D41" s="55"/>
+      <c r="E41" s="52" t="s">
         <v>56</v>
       </c>
-      <c r="F41" s="37"/>
-      <c r="G41" s="38"/>
+      <c r="F41" s="52"/>
+      <c r="G41" s="53"/>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B42" s="39" t="s">
+      <c r="B42" s="54" t="s">
         <v>49</v>
       </c>
-      <c r="C42" s="33"/>
-      <c r="D42" s="33"/>
-      <c r="E42" s="37" t="s">
+      <c r="C42" s="55"/>
+      <c r="D42" s="55"/>
+      <c r="E42" s="52" t="s">
         <v>56</v>
       </c>
-      <c r="F42" s="37"/>
-      <c r="G42" s="38"/>
+      <c r="F42" s="52"/>
+      <c r="G42" s="53"/>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B43" s="39" t="s">
+      <c r="B43" s="54" t="s">
         <v>49</v>
       </c>
-      <c r="C43" s="33"/>
-      <c r="D43" s="33"/>
-      <c r="E43" s="37" t="s">
+      <c r="C43" s="55"/>
+      <c r="D43" s="55"/>
+      <c r="E43" s="52" t="s">
         <v>56</v>
       </c>
-      <c r="F43" s="37"/>
-      <c r="G43" s="38"/>
+      <c r="F43" s="52"/>
+      <c r="G43" s="53"/>
     </row>
     <row r="44" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B44" s="61" t="s">
+      <c r="B44" s="72" t="s">
         <v>86</v>
       </c>
-      <c r="C44" s="62"/>
-      <c r="D44" s="62"/>
-      <c r="E44" s="63" t="s">
+      <c r="C44" s="73"/>
+      <c r="D44" s="73"/>
+      <c r="E44" s="74" t="s">
         <v>87</v>
       </c>
-      <c r="F44" s="63"/>
-      <c r="G44" s="64"/>
+      <c r="F44" s="74"/>
+      <c r="G44" s="75"/>
     </row>
   </sheetData>
   <mergeCells count="121">
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="F4:H4"/>
-    <mergeCell ref="R4:T4"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="F5:H5"/>
-    <mergeCell ref="R5:T5"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="Q2:T2"/>
-    <mergeCell ref="U2:W2"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="F3:H3"/>
-    <mergeCell ref="R3:T3"/>
-    <mergeCell ref="F2:N2"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="F6:H6"/>
-    <mergeCell ref="R6:T6"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="F7:H7"/>
-    <mergeCell ref="R7:T7"/>
-    <mergeCell ref="I6:K6"/>
-    <mergeCell ref="L6:N6"/>
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="L7:N7"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="F8:H8"/>
-    <mergeCell ref="R8:T8"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="F9:H9"/>
-    <mergeCell ref="R9:T9"/>
-    <mergeCell ref="I8:K8"/>
-    <mergeCell ref="L8:N8"/>
-    <mergeCell ref="I9:K9"/>
-    <mergeCell ref="L9:N9"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="F10:H10"/>
-    <mergeCell ref="R10:T10"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="O16:P16"/>
-    <mergeCell ref="Q16:S16"/>
-    <mergeCell ref="T16:V16"/>
-    <mergeCell ref="I10:K10"/>
-    <mergeCell ref="L10:N10"/>
-    <mergeCell ref="E20:G20"/>
-    <mergeCell ref="O20:P20"/>
-    <mergeCell ref="W16:Y16"/>
-    <mergeCell ref="AA16:AD16"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="E17:G17"/>
-    <mergeCell ref="O17:P17"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="E18:G18"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="AA24:AD24"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="E25:G25"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="E27:G27"/>
-    <mergeCell ref="Q22:AD22"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="O23:P23"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="E24:G24"/>
-    <mergeCell ref="O24:P24"/>
-    <mergeCell ref="Q24:S24"/>
-    <mergeCell ref="T24:V24"/>
-    <mergeCell ref="W24:Y24"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="E22:G22"/>
-    <mergeCell ref="O22:P22"/>
-    <mergeCell ref="I3:K3"/>
-    <mergeCell ref="L3:N3"/>
-    <mergeCell ref="I4:K4"/>
-    <mergeCell ref="L4:N4"/>
-    <mergeCell ref="I5:K5"/>
-    <mergeCell ref="L5:N5"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="E34:G34"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="E35:G35"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="E31:G31"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="E32:G32"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="E33:G33"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="E28:G28"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="E29:G29"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="E30:G30"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="E21:G21"/>
-    <mergeCell ref="B42:D42"/>
-    <mergeCell ref="E42:G42"/>
     <mergeCell ref="B43:D43"/>
     <mergeCell ref="E43:G43"/>
     <mergeCell ref="B44:D44"/>
@@ -3901,6 +3802,105 @@
     <mergeCell ref="E19:G19"/>
     <mergeCell ref="O19:P19"/>
     <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="E29:G29"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="E30:G30"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="E21:G21"/>
+    <mergeCell ref="B42:D42"/>
+    <mergeCell ref="E42:G42"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="E34:G34"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="E35:G35"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="E31:G31"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="E32:G32"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="E33:G33"/>
+    <mergeCell ref="AA24:AD24"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="E25:G25"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="E27:G27"/>
+    <mergeCell ref="Q22:AD22"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="O23:P23"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="O24:P24"/>
+    <mergeCell ref="Q24:S24"/>
+    <mergeCell ref="T24:V24"/>
+    <mergeCell ref="W24:Y24"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="E22:G22"/>
+    <mergeCell ref="O22:P22"/>
+    <mergeCell ref="E20:G20"/>
+    <mergeCell ref="O20:P20"/>
+    <mergeCell ref="W16:Y16"/>
+    <mergeCell ref="AA16:AD16"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="E17:G17"/>
+    <mergeCell ref="O17:P17"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="E18:G18"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="F10:H10"/>
+    <mergeCell ref="R10:T10"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="O16:P16"/>
+    <mergeCell ref="Q16:S16"/>
+    <mergeCell ref="T16:V16"/>
+    <mergeCell ref="I10:K10"/>
+    <mergeCell ref="L10:N10"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="F8:H8"/>
+    <mergeCell ref="R8:T8"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="F9:H9"/>
+    <mergeCell ref="R9:T9"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="L8:N8"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="L9:N9"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="F6:H6"/>
+    <mergeCell ref="R6:T6"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="F7:H7"/>
+    <mergeCell ref="R7:T7"/>
+    <mergeCell ref="I6:K6"/>
+    <mergeCell ref="L6:N6"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="L7:N7"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="R4:T4"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="R5:T5"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="Q2:T2"/>
+    <mergeCell ref="U2:W2"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="R3:T3"/>
+    <mergeCell ref="F2:N2"/>
+    <mergeCell ref="I3:K3"/>
+    <mergeCell ref="L3:N3"/>
+    <mergeCell ref="I4:K4"/>
+    <mergeCell ref="L4:N4"/>
+    <mergeCell ref="I5:K5"/>
+    <mergeCell ref="L5:N5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>